<commit_message>
Se libera version 1.2.0
</commit_message>
<xml_diff>
--- a/Programas/parametros.xlsx
+++ b/Programas/parametros.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="ton50ls" sheetId="1" r:id="rId1"/>
+    <sheet name="ton420ls" sheetId="2" r:id="rId1"/>
+    <sheet name="ton50ls" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>D750</t>
   </si>
@@ -238,6 +239,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:C34" totalsRowShown="0">
+  <autoFilter ref="A1:C34"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Registro"/>
+    <tableColumn id="2" name="Descripcion"/>
+    <tableColumn id="3" name="Valor"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C34" totalsRowShown="0">
   <autoFilter ref="A1:C34"/>
   <tableColumns count="3">
@@ -515,7 +528,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +555,354 @@
         <v>24</v>
       </c>
       <c r="C2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>21500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>21500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
         <v>2000</v>
       </c>
     </row>

</xml_diff>